<commit_message>
modify the interface to allow the conversion of all sheets and move to goRealeaser
</commit_message>
<xml_diff>
--- a/testdata/testfile2.xlsx
+++ b/testdata/testfile2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="23595" windowHeight="12780"/>
+    <workbookView xWindow="240" yWindow="36" windowWidth="23256" windowHeight="12780" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="5">
   <si>
     <t>Bob</t>
   </si>
@@ -70,7 +70,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -78,9 +78,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -118,7 +118,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -188,7 +188,7 @@
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -364,56 +364,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>
-        0
-      </v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>
-        1
-      </v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>
-        2
-      </v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>
-        3
-      </v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>
-        4
-      </v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>
-        3
-      </v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>
-        4
-      </v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>
-        3
-      </v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -423,12 +407,45 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -439,7 +456,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>